<commit_message>
busca pelo xls completa
</commit_message>
<xml_diff>
--- a/11.xlsx
+++ b/11.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="77">
   <si>
     <t xml:space="preserve">et_title_product_id</t>
   </si>
@@ -178,6 +178,9 @@
     <t xml:space="preserve">4</t>
   </si>
   <si>
+    <t xml:space="preserve">21654646546</t>
+  </si>
+  <si>
     <t xml:space="preserve">teste teste</t>
   </si>
   <si>
@@ -185,6 +188,69 @@
   </si>
   <si>
     <t xml:space="preserve">Fsxxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18828831570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolsa Feminina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">211492050758</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96030C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119.90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18828821908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">163867386648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12003A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">149.90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">163867386649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">163867386650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">163867386651</t>
+  </si>
+  <si>
+    <t xml:space="preserve">163867386652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">163867386653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18828809899</t>
   </si>
 </sst>
 </file>
@@ -197,7 +263,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -247,6 +313,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -307,7 +379,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,6 +429,10 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,10 +516,10 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B25" activeCellId="0" sqref="B25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.03125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1013,18 +1089,18 @@
       <c r="Z16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
+      <c r="A17" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="B17" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D17" s="6"/>
       <c r="E17" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8" t="s">
@@ -1051,6 +1127,174 @@
       <c r="X17" s="11"/>
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="1046380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1046381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3250,7 +3494,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <dataValidations count="24">
+  <dataValidations count="40">
     <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G5" type="custom">
       <formula1>AND(G5&gt;=1,G5&lt;=100000,LEN($G5)-LEN(INT($G5))-1&lt;=2)</formula1>
       <formula2>0</formula2>
@@ -3345,6 +3589,70 @@
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H16" type="custom">
       <formula1>AND(H16&gt;=0,H16&lt;=10000000,LEN($H16)-LEN(INT($H16))&lt;=0)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G18" type="custom">
+      <formula1>AND(G43&gt;=1,G43&lt;=100000,LEN($G43)-LEN(INT($G43))-1&lt;=2)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G19" type="custom">
+      <formula1>AND(G44&gt;=1,G44&lt;=100000,LEN($G44)-LEN(INT($G44))-1&lt;=2)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G20" type="custom">
+      <formula1>AND(G45&gt;=1,G45&lt;=100000,LEN($G45)-LEN(INT($G45))-1&lt;=2)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G21" type="custom">
+      <formula1>AND(G46&gt;=1,G46&lt;=100000,LEN($G46)-LEN(INT($G46))-1&lt;=2)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G22" type="custom">
+      <formula1>AND(G47&gt;=1,G47&lt;=100000,LEN($G47)-LEN(INT($G47))-1&lt;=2)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G23" type="custom">
+      <formula1>AND(G48&gt;=1,G48&lt;=100000,LEN($G48)-LEN(INT($G48))-1&lt;=2)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G24" type="custom">
+      <formula1>AND(G49&gt;=1,G49&lt;=100000,LEN($G49)-LEN(INT($G49))-1&lt;=2)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G25" type="custom">
+      <formula1>AND(G50&gt;=1,G50&lt;=100000,LEN($G50)-LEN(INT($G50))-1&lt;=2)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H18" type="custom">
+      <formula1>AND(H43&gt;=0,H43&lt;=10000000,LEN($H43)-LEN(INT($H43))&lt;=0)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H19" type="custom">
+      <formula1>AND(H44&gt;=0,H44&lt;=10000000,LEN($H44)-LEN(INT($H44))&lt;=0)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H20" type="custom">
+      <formula1>AND(H45&gt;=0,H45&lt;=10000000,LEN($H45)-LEN(INT($H45))&lt;=0)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H21" type="custom">
+      <formula1>AND(H46&gt;=0,H46&lt;=10000000,LEN($H46)-LEN(INT($H46))&lt;=0)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H22" type="custom">
+      <formula1>AND(H47&gt;=0,H47&lt;=10000000,LEN($H47)-LEN(INT($H47))&lt;=0)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H23" type="custom">
+      <formula1>AND(H48&gt;=0,H48&lt;=10000000,LEN($H48)-LEN(INT($H48))&lt;=0)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H24" type="custom">
+      <formula1>AND(H49&gt;=0,H49&lt;=10000000,LEN($H49)-LEN(INT($H49))&lt;=0)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H25" type="custom">
+      <formula1>AND(H50&gt;=0,H50&lt;=10000000,LEN($H50)-LEN(INT($H50))&lt;=0)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>